<commit_message>
SP rentalhousedetails is in progress
</commit_message>
<xml_diff>
--- a/PropertyDocu/Property.xlsx
+++ b/PropertyDocu/Property.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="65">
   <si>
     <t>S.No</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t>Rental Occupied</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -590,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,7 +630,7 @@
         <v>3</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
PaymentForRent and Scheme SP are created
</commit_message>
<xml_diff>
--- a/PropertyDocu/Property.xlsx
+++ b/PropertyDocu/Property.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="88">
   <si>
     <t>S.No</t>
   </si>
@@ -217,9 +217,6 @@
     <t>enable Verified</t>
   </si>
   <si>
-    <t>Verified</t>
-  </si>
-  <si>
     <t>Phone 1 (Primary Contact)</t>
   </si>
   <si>
@@ -230,6 +227,78 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Pets Allowed</t>
+  </si>
+  <si>
+    <t>Rent From</t>
+  </si>
+  <si>
+    <t>Rent To</t>
+  </si>
+  <si>
+    <t>Phone Verified</t>
+  </si>
+  <si>
+    <t>Payment For Rent</t>
+  </si>
+  <si>
+    <t>HouseOwnerId</t>
+  </si>
+  <si>
+    <t>RentHouseId</t>
+  </si>
+  <si>
+    <t>PaymentDate</t>
+  </si>
+  <si>
+    <t>PaymentReceivedDate</t>
+  </si>
+  <si>
+    <t>Scheme</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>SchemeName</t>
+  </si>
+  <si>
+    <t>SchemeDuration</t>
+  </si>
+  <si>
+    <t>DiscountPercentage</t>
+  </si>
+  <si>
+    <t>SchemeId</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>AmountPaid</t>
+  </si>
+  <si>
+    <t>ReferenceNumber</t>
+  </si>
+  <si>
+    <t>BankDetails</t>
+  </si>
+  <si>
+    <t>TransactionSuccessfull</t>
+  </si>
+  <si>
+    <t>Rental</t>
+  </si>
+  <si>
+    <t>TenantId</t>
+  </si>
+  <si>
+    <t>Payment For Tenant</t>
+  </si>
+  <si>
+    <t>Tenant</t>
   </si>
 </sst>
 </file>
@@ -591,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,14 +674,18 @@
     <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="37" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="37" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -630,10 +703,19 @@
         <v>3</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -652,8 +734,17 @@
       <c r="I3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" t="s">
+        <v>74</v>
+      </c>
+      <c r="M3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -669,8 +760,17 @@
       <c r="I4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -686,8 +786,17 @@
       <c r="I5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>71</v>
+      </c>
+      <c r="L5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>39</v>
       </c>
@@ -697,8 +806,17 @@
       <c r="I6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>72</v>
+      </c>
+      <c r="L6" t="s">
+        <v>77</v>
+      </c>
+      <c r="M6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>20</v>
       </c>
@@ -706,12 +824,21 @@
         <v>16</v>
       </c>
       <c r="I7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="J7" t="s">
+        <v>80</v>
+      </c>
+      <c r="L7" t="s">
+        <v>79</v>
+      </c>
+      <c r="M7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G8" t="s">
         <v>17</v>
@@ -719,8 +846,17 @@
       <c r="I8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>78</v>
+      </c>
+      <c r="L8" t="s">
+        <v>84</v>
+      </c>
+      <c r="M8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>21</v>
       </c>
@@ -730,8 +866,17 @@
       <c r="I9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>81</v>
+      </c>
+      <c r="L9" t="s">
+        <v>87</v>
+      </c>
+      <c r="M9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>22</v>
       </c>
@@ -741,8 +886,14 @@
       <c r="I10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>82</v>
+      </c>
+      <c r="M10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>23</v>
       </c>
@@ -752,8 +903,11 @@
       <c r="I11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>24</v>
       </c>
@@ -764,7 +918,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>27</v>
       </c>
@@ -775,7 +929,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>28</v>
       </c>
@@ -786,7 +940,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>12</v>
       </c>
@@ -797,7 +951,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>13</v>
       </c>
@@ -854,7 +1008,22 @@
         <v>19</v>
       </c>
       <c r="I21" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -868,7 +1037,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,7 +1171,7 @@
         <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="G7" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
login coded updated, login tbl
</commit_message>
<xml_diff>
--- a/PropertyDocu/Property.xlsx
+++ b/PropertyDocu/Property.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="106">
   <si>
     <t>S.No</t>
   </si>
@@ -299,6 +299,60 @@
   </si>
   <si>
     <t>Tenant</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>EmailID</t>
+  </si>
+  <si>
+    <t>PhoneNumberVerified</t>
+  </si>
+  <si>
+    <t>EmailIdVerified</t>
+  </si>
+  <si>
+    <t>PhoneNumberCode</t>
+  </si>
+  <si>
+    <t>CodeSendDate</t>
+  </si>
+  <si>
+    <t>ExipryTime</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>EMailCode</t>
+  </si>
+  <si>
+    <t>CodeSendTime</t>
+  </si>
+  <si>
+    <t>LoginID</t>
+  </si>
+  <si>
+    <t>ReVerificationTime</t>
+  </si>
+  <si>
+    <t>PhoneNumberVerifiedDate</t>
+  </si>
+  <si>
+    <t>EmailIdVerifiedDate</t>
+  </si>
+  <si>
+    <t>MandatoryVerification</t>
+  </si>
+  <si>
+    <t>ReVerification</t>
   </si>
 </sst>
 </file>
@@ -660,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,14 +732,16 @@
     <col min="11" max="11" width="10.7109375" customWidth="1"/>
     <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -714,8 +770,14 @@
       <c r="M2" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -743,8 +805,14 @@
       <c r="M3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>74</v>
+      </c>
+      <c r="P3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -769,8 +837,14 @@
       <c r="M4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O4" t="s">
+        <v>88</v>
+      </c>
+      <c r="P4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -795,8 +869,14 @@
       <c r="M5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O5" t="s">
+        <v>46</v>
+      </c>
+      <c r="P5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>39</v>
       </c>
@@ -815,8 +895,14 @@
       <c r="M6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O6" t="s">
+        <v>69</v>
+      </c>
+      <c r="P6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>20</v>
       </c>
@@ -835,8 +921,14 @@
       <c r="M7" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>85</v>
+      </c>
+      <c r="P7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>60</v>
       </c>
@@ -855,8 +947,14 @@
       <c r="M8" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O8" t="s">
+        <v>89</v>
+      </c>
+      <c r="P8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>21</v>
       </c>
@@ -875,8 +973,14 @@
       <c r="M9" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O9" t="s">
+        <v>90</v>
+      </c>
+      <c r="P9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>22</v>
       </c>
@@ -892,8 +996,14 @@
       <c r="M10" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O10" t="s">
+        <v>91</v>
+      </c>
+      <c r="P10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>23</v>
       </c>
@@ -906,8 +1016,14 @@
       <c r="J11" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O11" t="s">
+        <v>92</v>
+      </c>
+      <c r="P11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>24</v>
       </c>
@@ -917,8 +1033,14 @@
       <c r="I12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O12" t="s">
+        <v>101</v>
+      </c>
+      <c r="P12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>27</v>
       </c>
@@ -928,8 +1050,11 @@
       <c r="I13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>28</v>
       </c>
@@ -939,8 +1064,11 @@
       <c r="I14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>12</v>
       </c>
@@ -950,8 +1078,11 @@
       <c r="I15" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>13</v>
       </c>
@@ -960,6 +1091,9 @@
       </c>
       <c r="I16" t="s">
         <v>33</v>
+      </c>
+      <c r="O16" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="5:9" x14ac:dyDescent="0.25">

</xml_diff>